<commit_message>
Se creo funcion rellenar... en modulo para rellenar csv una vez el feeder se calibre
</commit_message>
<xml_diff>
--- a/mantto_feeder.xlsx
+++ b/mantto_feeder.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="15840" windowWidth="29040" xWindow="-120" yWindow="-120"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="11385" windowWidth="21600" xWindow="0" yWindow="3060"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
@@ -422,16 +422,16 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V17"/>
+  <dimension ref="A1:W17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q3" sqref="Q3"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="J9" sqref="J9:V9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col customWidth="1" max="1" min="1" style="3" width="20"/>
-    <col bestFit="1" customWidth="1" max="2" min="2" style="3" width="13"/>
+    <col bestFit="1" customWidth="1" max="2" min="2" style="3" width="17.28515625"/>
   </cols>
   <sheetData>
     <row customHeight="1" ht="26.25" r="1" s="3">
@@ -667,11 +667,78 @@
         </is>
       </c>
     </row>
-    <row r="5"/>
-    <row r="6"/>
-    <row r="7"/>
-    <row r="8"/>
-    <row r="9"/>
+    <row r="9">
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="L9" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="M9" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="N9" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="O9" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="P9" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="Q9" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="R9" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="S9" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="T9" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="U9" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="V9" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="W9" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+    </row>
     <row r="10"/>
     <row r="11"/>
     <row r="12"/>

</xml_diff>